<commit_message>
Added feature to eliminate duplicate tweets
</commit_message>
<xml_diff>
--- a/titles.xlsx
+++ b/titles.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -29,6 +29,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -113,17 +114,17 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A1:A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>